<commit_message>
website interface improvement. Fit in the database, added 4 columns. Adjust the business rule.
</commit_message>
<xml_diff>
--- a/ModuleGenerateCSV/StrutureData0.xlsx
+++ b/ModuleGenerateCSV/StrutureData0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MDS\MedicalDecisionSupport\ModuleGenerateCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C4CC86-AA57-424D-BDA2-4669222DE3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0BADB7-CC60-4FAA-8F22-3B2CA9186DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{97C584F9-C9E0-4BA7-80FE-11BDE73D0544}"/>
   </bookViews>
@@ -361,6 +361,9 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -375,9 +378,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,7 +823,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,43 +847,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="5" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="27"/>
-      <c r="K1" s="23" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="26"/>
     </row>
     <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
       <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
@@ -985,7 +985,10 @@
         <f t="shared" ref="M4:M13" si="0">SUM(C4:H4)</f>
         <v>7</v>
       </c>
-      <c r="N4" s="28"/>
+      <c r="N4" s="23">
+        <f>SUM(K4+L4+M4)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
@@ -1029,6 +1032,10 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
+      <c r="N5" s="23">
+        <f t="shared" ref="N5:N13" si="1">SUM(K5+L5+M5)</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
@@ -1072,6 +1079,10 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="N6" s="23">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -1115,6 +1126,10 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="N7" s="23">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
@@ -1158,6 +1173,10 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="N8" s="23">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
@@ -1201,6 +1220,10 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
+      <c r="N9" s="23">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
@@ -1244,7 +1267,10 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="N10" s="19"/>
+      <c r="N10" s="23">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
       <c r="O10" s="19"/>
       <c r="P10" s="19"/>
       <c r="Q10" s="19"/>
@@ -1291,7 +1317,10 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="N11" s="18"/>
+      <c r="N11" s="23">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
       <c r="O11" s="22"/>
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
@@ -1338,7 +1367,10 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="N12" s="18"/>
+      <c r="N12" s="23">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
       <c r="O12" s="22"/>
       <c r="P12" s="18"/>
       <c r="Q12" s="18"/>
@@ -1385,7 +1417,10 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="N13" s="18"/>
+      <c r="N13" s="23">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
       <c r="O13" s="22"/>
       <c r="P13" s="18"/>
       <c r="Q13" s="18"/>

</xml_diff>